<commit_message>
Updated IPC and init graphs
</commit_message>
<xml_diff>
--- a/graphs/Project-Graphs.xlsx
+++ b/graphs/Project-Graphs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="899" firstSheet="8" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="899" firstSheet="5" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-anagram Before" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="20">
   <si>
     <t>2-level</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>% Extraneous Branches</t>
+  </si>
+  <si>
+    <t>IPC %</t>
   </si>
 </sst>
 </file>
@@ -163,8 +166,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -186,17 +201,29 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -316,11 +343,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2080615288"/>
-        <c:axId val="2080612296"/>
+        <c:axId val="2076617896"/>
+        <c:axId val="2074956168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2080615288"/>
+        <c:axId val="2076617896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -339,7 +366,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2080612296"/>
+        <c:crossAx val="2074956168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -347,7 +374,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2080612296"/>
+        <c:axId val="2074956168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -368,7 +395,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2080615288"/>
+        <c:crossAx val="2076617896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -405,7 +432,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2800"/>
-              <a:t>IPC vs Initial Confidence Table Entry Value for compress Benchmark</a:t>
+              <a:t>% IPC vs Initial Confidence Table Entry Value for compress Benchmark</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -434,30 +461,28 @@
             </c:strRef>
           </c:tx>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Final Results'!$B$31:$G$31</c:f>
+              <c:f>'Final Results'!$C$43:$G$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.0</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>45.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -465,27 +490,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Final Results'!$B$34:$G$34</c:f>
+              <c:f>'Final Results'!$C$46:$G$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.6489</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>99.93935350839953</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6479</c:v>
+                  <c:v>99.93328885923948</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6478</c:v>
+                  <c:v>99.89083631511917</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6471</c:v>
+                  <c:v>99.95754745587967</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6482</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.6477</c:v>
+                  <c:v>99.92722421007944</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -502,11 +524,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2123124872"/>
-        <c:axId val="-2122408680"/>
+        <c:axId val="2075899384"/>
+        <c:axId val="2075904952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2123124872"/>
+        <c:axId val="2075899384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -545,7 +567,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122408680"/>
+        <c:crossAx val="2075904952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -553,7 +575,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122408680"/>
+        <c:axId val="2075904952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -571,7 +593,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="2400"/>
-                  <a:t>IPC</a:t>
+                  <a:t>% IPC</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -593,7 +615,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2123124872"/>
+        <c:crossAx val="2075899384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -630,7 +652,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2800"/>
-              <a:t>IPC vs Initial Confidence Table</a:t>
+              <a:t>% IPC vs Initial Confidence Table</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="2800" baseline="0"/>
@@ -664,30 +686,28 @@
             </c:strRef>
           </c:tx>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Final Results'!$B$31:$G$31</c:f>
+              <c:f>'Final Results'!$C$43:$G$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.0</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>45.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -695,27 +715,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Final Results'!$B$35:$G$35</c:f>
+              <c:f>'Final Results'!$C$47:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.3762</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100.2923976608187</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3773</c:v>
+                  <c:v>100.3455608718767</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3775</c:v>
+                  <c:v>100.3189792663477</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.3774</c:v>
+                  <c:v>100.3189792663477</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3774</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.3774</c:v>
+                  <c:v>100.3189792663477</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -732,11 +749,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2124168120"/>
-        <c:axId val="2134901096"/>
+        <c:axId val="2075942328"/>
+        <c:axId val="2075948120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2124168120"/>
+        <c:axId val="2075942328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -780,7 +797,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134901096"/>
+        <c:crossAx val="2075948120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -788,9 +805,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2134901096"/>
+        <c:axId val="2075948120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="100.28"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -806,7 +824,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="2400"/>
-                  <a:t>IPC</a:t>
+                  <a:t>% IPC</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -828,7 +846,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2124168120"/>
+        <c:crossAx val="2075942328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -865,7 +883,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2800"/>
-              <a:t>IPC vs Confidence Level for gcc Benchmark</a:t>
+              <a:t>% IPC vs Confidence Level for gcc Benchmark</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -897,26 +915,23 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Final Results'!$B$1:$G$1</c:f>
+              <c:f>'Final Results'!$C$37:$G$37</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>0.75</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.0%">
+                <c:pt idx="2" formatCode="0.0%">
                   <c:v>0.875</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="3">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.00%">
+                <c:pt idx="4" formatCode="0.00%">
                   <c:v>0.9375</c:v>
                 </c:pt>
               </c:numCache>
@@ -924,27 +939,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Final Results'!$B$2:$G$2</c:f>
+              <c:f>'Final Results'!$C$38:$G$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.1145</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>98.21444593988334</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0946</c:v>
+                  <c:v>100.4037685060565</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.119</c:v>
+                  <c:v>101.2202781516375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1281</c:v>
+                  <c:v>101.2382234185734</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1283</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1268</c:v>
+                  <c:v>101.1036339165545</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -959,11 +971,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="2093424424"/>
-        <c:axId val="-2136439080"/>
+        <c:axId val="2076644072"/>
+        <c:axId val="2076649656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2093424424"/>
+        <c:axId val="2076644072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1002,7 +1014,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2136439080"/>
+        <c:crossAx val="2076649656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1010,7 +1022,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2136439080"/>
+        <c:axId val="2076649656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1028,7 +1040,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="2400"/>
-                  <a:t>IPC</a:t>
+                  <a:t>% IPC</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1050,9 +1062,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2093424424"/>
+        <c:crossAx val="2076644072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="0.5"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -1087,7 +1100,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2800"/>
-              <a:t>IPC vs Confidence Level for go Benchmark</a:t>
+              <a:t>% IPC vs Confidence Level for go Benchmark</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1119,26 +1132,23 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Final Results'!$B$1:$G$1</c:f>
+              <c:f>'Final Results'!$C$37:$G$37</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>0.75</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.0%">
+                <c:pt idx="2" formatCode="0.0%">
                   <c:v>0.875</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="3">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.00%">
+                <c:pt idx="4" formatCode="0.00%">
                   <c:v>0.9375</c:v>
                 </c:pt>
               </c:numCache>
@@ -1146,27 +1156,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Final Results'!$B$3:$G$3</c:f>
+              <c:f>'Final Results'!$C$39:$G$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.2035</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>103.2405484004985</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2425</c:v>
+                  <c:v>104.3955130868301</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2564</c:v>
+                  <c:v>104.0548400498546</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2523</c:v>
+                  <c:v>103.9551308683008</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2511</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.2495</c:v>
+                  <c:v>103.8221852928957</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1181,11 +1188,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="-2134455944"/>
-        <c:axId val="-2134762904"/>
+        <c:axId val="2076668200"/>
+        <c:axId val="2076673864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2134455944"/>
+        <c:axId val="2076668200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1224,7 +1231,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2134762904"/>
+        <c:crossAx val="2076673864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1232,10 +1239,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2134762904"/>
+        <c:axId val="2076673864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="1.17"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1251,7 +1257,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="2400"/>
-                  <a:t>IPC</a:t>
+                  <a:t>% IPC</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1273,10 +1279,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2134455944"/>
+        <c:crossAx val="2076668200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.02"/>
+        <c:majorUnit val="0.25"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -1311,7 +1317,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2800"/>
-              <a:t>IPC vs Confidence Level for compress Benchmark</a:t>
+              <a:t>% IPC vs Confidence Level for compress Benchmark</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1343,26 +1349,23 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Final Results'!$B$1:$G$1</c:f>
+              <c:f>'Final Results'!$C$37:$G$37</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>0.75</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.0%">
+                <c:pt idx="2" formatCode="0.0%">
                   <c:v>0.875</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="3">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.00%">
+                <c:pt idx="4" formatCode="0.00%">
                   <c:v>0.9375</c:v>
                 </c:pt>
               </c:numCache>
@@ -1370,27 +1373,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Final Results'!$B$4:$G$4</c:f>
+              <c:f>'Final Results'!$C$40:$G$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.804</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>91.44678492239467</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6497</c:v>
+                  <c:v>91.44678492239467</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6497</c:v>
+                  <c:v>91.39689578713968</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6488</c:v>
+                  <c:v>91.40243902439024</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6489</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.6485</c:v>
+                  <c:v>91.38026607538802</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1405,11 +1405,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="-2131982104"/>
-        <c:axId val="-2126706904"/>
+        <c:axId val="2076026168"/>
+        <c:axId val="2076031944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2131982104"/>
+        <c:axId val="2076026168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1453,7 +1453,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2126706904"/>
+        <c:crossAx val="2076031944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1461,7 +1461,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2126706904"/>
+        <c:axId val="2076031944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1479,7 +1479,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="2400"/>
-                  <a:t>IPC</a:t>
+                  <a:t>% IPC</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1501,7 +1501,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131982104"/>
+        <c:crossAx val="2076026168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1538,7 +1538,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2800"/>
-              <a:t>IPC vs Confidence Level for anagram</a:t>
+              <a:t>% IPC vs Confidence Level for anagram</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="2800" baseline="0"/>
@@ -1575,26 +1575,23 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Final Results'!$B$1:$G$1</c:f>
+              <c:f>'Final Results'!$C$37:$G$37</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>0.75</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.0%">
+                <c:pt idx="2" formatCode="0.0%">
                   <c:v>0.875</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="3">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.00%">
+                <c:pt idx="4" formatCode="0.00%">
                   <c:v>0.9375</c:v>
                 </c:pt>
               </c:numCache>
@@ -1602,27 +1599,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Final Results'!$B$5:$G$5</c:f>
+              <c:f>'Final Results'!$C$41:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.3743</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100.7213465134919</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.377</c:v>
+                  <c:v>100.4808976756612</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3761</c:v>
+                  <c:v>100.4541811381245</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.376</c:v>
+                  <c:v>100.507614213198</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3762</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.3759</c:v>
+                  <c:v>100.4274646005878</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1637,11 +1631,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="-2125585048"/>
-        <c:axId val="-2126057304"/>
+        <c:axId val="2076069192"/>
+        <c:axId val="2076074728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2125585048"/>
+        <c:axId val="2076069192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1680,7 +1674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2126057304"/>
+        <c:crossAx val="2076074728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1688,7 +1682,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2126057304"/>
+        <c:axId val="2076074728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1706,7 +1700,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="2400"/>
-                  <a:t>IPC</a:t>
+                  <a:t>% IPC</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1728,10 +1722,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125585048"/>
+        <c:crossAx val="2076069192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.001"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -2021,11 +2014,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2138369896"/>
-        <c:axId val="2138454104"/>
+        <c:axId val="2076120584"/>
+        <c:axId val="2076126088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2138369896"/>
+        <c:axId val="2076120584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2054,7 +2047,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2138454104"/>
+        <c:crossAx val="2076126088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2062,7 +2055,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2138454104"/>
+        <c:axId val="2076126088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.2"/>
@@ -2094,7 +2087,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2138369896"/>
+        <c:crossAx val="2076120584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.01"/>
@@ -2181,7 +2174,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2431,11 +2423,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2082583848"/>
-        <c:axId val="-2137041864"/>
+        <c:axId val="2075475032"/>
+        <c:axId val="2075469528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2082583848"/>
+        <c:axId val="2075475032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2457,14 +2449,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137041864"/>
+        <c:crossAx val="2075469528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2472,7 +2463,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2137041864"/>
+        <c:axId val="2075469528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.27"/>
@@ -2497,14 +2488,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082583848"/>
+        <c:crossAx val="2075475032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.015"/>
@@ -2591,7 +2581,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2841,11 +2830,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2136371384"/>
-        <c:axId val="-2136368280"/>
+        <c:axId val="2075421992"/>
+        <c:axId val="2075416488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2136371384"/>
+        <c:axId val="2075421992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2867,14 +2856,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136368280"/>
+        <c:crossAx val="2075416488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2882,7 +2870,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2136368280"/>
+        <c:axId val="2075416488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2905,14 +2893,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136371384"/>
+        <c:crossAx val="2075421992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2998,7 +2985,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3248,11 +3234,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2137998984"/>
-        <c:axId val="-2137965000"/>
+        <c:axId val="2048221064"/>
+        <c:axId val="2048215576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2137998984"/>
+        <c:axId val="2048221064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3274,14 +3260,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137965000"/>
+        <c:crossAx val="2048215576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3289,7 +3274,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2137965000"/>
+        <c:axId val="2048215576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.04"/>
@@ -3313,14 +3298,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137998984"/>
+        <c:crossAx val="2048221064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3411,7 +3395,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3544,11 +3527,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2029937176"/>
-        <c:axId val="2029969544"/>
+        <c:axId val="2074972360"/>
+        <c:axId val="2074975368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2029937176"/>
+        <c:axId val="2074972360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3567,7 +3550,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2029969544"/>
+        <c:crossAx val="2074975368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3575,7 +3558,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2029969544"/>
+        <c:axId val="2074975368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3596,14 +3579,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2029937176"/>
+        <c:crossAx val="2074972360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3933,11 +3915,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2084500056"/>
-        <c:axId val="2086475320"/>
+        <c:axId val="2074435688"/>
+        <c:axId val="2074432488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2084500056"/>
+        <c:axId val="2074435688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3947,7 +3929,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086475320"/>
+        <c:crossAx val="2074432488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3955,7 +3937,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2086475320"/>
+        <c:axId val="2074432488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3966,14 +3948,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2084500056"/>
+        <c:crossAx val="2074435688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4355,11 +4336,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2089404168"/>
-        <c:axId val="2089407224"/>
+        <c:axId val="2048117336"/>
+        <c:axId val="2048114184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2089404168"/>
+        <c:axId val="2048117336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4368,7 +4349,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2089407224"/>
+        <c:crossAx val="2048114184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4376,7 +4357,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2089407224"/>
+        <c:axId val="2048114184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4387,14 +4368,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2089404168"/>
+        <c:crossAx val="2048117336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4571,11 +4551,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2080565048"/>
-        <c:axId val="2080560856"/>
+        <c:axId val="2048861640"/>
+        <c:axId val="2048864664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2080565048"/>
+        <c:axId val="2048861640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4594,7 +4574,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2080560856"/>
+        <c:crossAx val="2048864664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4602,7 +4582,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2080560856"/>
+        <c:axId val="2048864664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4623,7 +4603,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2080565048"/>
+        <c:crossAx val="2048861640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4775,8 +4755,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2089396664"/>
-        <c:axId val="2094208520"/>
+        <c:axId val="2075031016"/>
+        <c:axId val="2075056616"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4871,11 +4851,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2134711576"/>
-        <c:axId val="2091068440"/>
+        <c:axId val="2075067800"/>
+        <c:axId val="2075062344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2089396664"/>
+        <c:axId val="2075031016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4904,7 +4884,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2094208520"/>
+        <c:crossAx val="2075056616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4912,7 +4892,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2094208520"/>
+        <c:axId val="2075056616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4942,12 +4922,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2089396664"/>
+        <c:crossAx val="2075031016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2091068440"/>
+        <c:axId val="2075062344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4976,12 +4956,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134711576"/>
+        <c:crossAx val="2075067800"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2134711576"/>
+        <c:axId val="2075067800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4991,7 +4971,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091068440"/>
+        <c:crossAx val="2075062344"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -5079,7 +5060,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5175,8 +5155,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2138964008"/>
-        <c:axId val="2138967080"/>
+        <c:axId val="2075075784"/>
+        <c:axId val="2075081256"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5268,11 +5248,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2133671656"/>
-        <c:axId val="2136800120"/>
+        <c:axId val="2075092488"/>
+        <c:axId val="2075086984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2138964008"/>
+        <c:axId val="2075075784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5294,14 +5274,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2138967080"/>
+        <c:crossAx val="2075081256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5309,7 +5288,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2138967080"/>
+        <c:axId val="2075081256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5332,19 +5311,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2138964008"/>
+        <c:crossAx val="2075075784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2136800120"/>
+        <c:axId val="2075086984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5366,20 +5344,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133671656"/>
+        <c:crossAx val="2075092488"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.02"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2133671656"/>
+        <c:axId val="2075092488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5389,7 +5366,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2136800120"/>
+        <c:crossAx val="2075086984"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -5477,7 +5455,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5573,8 +5550,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2088872056"/>
-        <c:axId val="2138495800"/>
+        <c:axId val="2075692424"/>
+        <c:axId val="2075697896"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5666,11 +5643,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2138344248"/>
-        <c:axId val="2138341448"/>
+        <c:axId val="2075709016"/>
+        <c:axId val="2075703528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2088872056"/>
+        <c:axId val="2075692424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5692,14 +5669,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2138495800"/>
+        <c:crossAx val="2075697896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5707,7 +5683,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2138495800"/>
+        <c:axId val="2075697896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5730,19 +5706,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088872056"/>
+        <c:crossAx val="2075692424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2138341448"/>
+        <c:axId val="2075703528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5764,19 +5739,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2138344248"/>
+        <c:crossAx val="2075709016"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2138344248"/>
+        <c:axId val="2075709016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5786,7 +5760,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2138341448"/>
+        <c:crossAx val="2075703528"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -5874,7 +5849,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5970,8 +5944,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2138065512"/>
-        <c:axId val="2138336792"/>
+        <c:axId val="2075760600"/>
+        <c:axId val="2075766088"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6063,11 +6037,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2134641944"/>
-        <c:axId val="2137957672"/>
+        <c:axId val="2075777208"/>
+        <c:axId val="2075771720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2138065512"/>
+        <c:axId val="2075760600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6089,14 +6063,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2138336792"/>
+        <c:crossAx val="2075766088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6104,7 +6077,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2138336792"/>
+        <c:axId val="2075766088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6127,19 +6100,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2138065512"/>
+        <c:crossAx val="2075760600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2137957672"/>
+        <c:axId val="2075771720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6161,20 +6133,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134641944"/>
+        <c:crossAx val="2075777208"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.001"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2134641944"/>
+        <c:axId val="2075777208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6184,7 +6155,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137957672"/>
+        <c:crossAx val="2075771720"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -6267,7 +6239,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2800"/>
-              <a:t>IPC vs Initial Confidence</a:t>
+              <a:t>% IPC vs Initial Confidence</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="2800" baseline="0"/>
@@ -6301,30 +6273,28 @@
             </c:strRef>
           </c:tx>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Final Results'!$B$31:$G$31</c:f>
+              <c:f>'Final Results'!$C$43:$G$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.0</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>45.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -6332,27 +6302,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Final Results'!$B$32:$G$32</c:f>
+              <c:f>'Final Results'!$C$44:$G$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.1283</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100.2127093858016</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1307</c:v>
+                  <c:v>100.2747496233271</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1314</c:v>
+                  <c:v>100.3102011876274</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1318</c:v>
+                  <c:v>100.3279269697775</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.132</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1322</c:v>
+                  <c:v>100.3456527519277</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6369,11 +6336,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2130501208"/>
-        <c:axId val="-2122764920"/>
+        <c:axId val="2075808904"/>
+        <c:axId val="2075814696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2130501208"/>
+        <c:axId val="2075808904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6417,7 +6384,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122764920"/>
+        <c:crossAx val="2075814696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6425,7 +6392,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122764920"/>
+        <c:axId val="2075814696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6443,8 +6410,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="2400"/>
+                  <a:t>% </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2400" baseline="0"/>
                   <a:t>IPC</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-US" sz="2400"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -6465,7 +6437,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2130501208"/>
+        <c:crossAx val="2075808904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6502,7 +6474,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2800"/>
-              <a:t>IPC vs Initial Confidence Table Entry Value for go</a:t>
+              <a:t>% IPC vs Initial Confidence Table Entry Value for go</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="2800" baseline="0"/>
@@ -6536,30 +6508,28 @@
             </c:strRef>
           </c:tx>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Final Results'!$B$31:$G$31</c:f>
+              <c:f>'Final Results'!$C$43:$G$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.0</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>45.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -6567,27 +6537,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Final Results'!$B$33:$G$33</c:f>
+              <c:f>'Final Results'!$C$45:$G$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.2511</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100.095915594277</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2523</c:v>
+                  <c:v>100.0399648309488</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2516</c:v>
+                  <c:v>100.0079929661898</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2512</c:v>
+                  <c:v>99.97602110143072</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2508</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.2505</c:v>
+                  <c:v>99.95204220286146</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6604,11 +6571,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2123201192"/>
-        <c:axId val="-2123143640"/>
+        <c:axId val="2075855496"/>
+        <c:axId val="2075861064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2123201192"/>
+        <c:axId val="2075855496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6647,7 +6614,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2123143640"/>
+        <c:crossAx val="2075861064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6655,7 +6622,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2123143640"/>
+        <c:axId val="2075861064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6673,7 +6640,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="2400"/>
-                  <a:t>IPC</a:t>
+                  <a:t>% IPC</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6695,7 +6662,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2123201192"/>
+        <c:crossAx val="2075855496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6777,7 +6744,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="122" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="122" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -6788,7 +6755,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="122" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="122" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -7131,7 +7098,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8575989" cy="5833626"/>
+    <xdr:ext cx="8567295" cy="5829508"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -7347,7 +7314,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8575989" cy="5833626"/>
+    <xdr:ext cx="8567295" cy="5829508"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -8000,10 +7967,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView showRuler="0" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8702,6 +8669,276 @@
         <v>0.37740000000000001</v>
       </c>
     </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="4">
+        <v>0</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="F37" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="G37" s="5">
+        <v>0.9375</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <v>1.1145</v>
+      </c>
+      <c r="C38">
+        <f>C2/B2*100</f>
+        <v>98.214445939883348</v>
+      </c>
+      <c r="D38">
+        <f>D2/B2*100</f>
+        <v>100.40376850605652</v>
+      </c>
+      <c r="E38">
+        <f>E2/B2*100</f>
+        <v>101.22027815163752</v>
+      </c>
+      <c r="F38">
+        <f>F2/B2*100</f>
+        <v>101.23822341857336</v>
+      </c>
+      <c r="G38">
+        <f>G2/B2*100</f>
+        <v>101.1036339165545</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="7">
+        <v>1.2035</v>
+      </c>
+      <c r="C39">
+        <f>C3/B3*100</f>
+        <v>103.24054840049854</v>
+      </c>
+      <c r="D39">
+        <f>D3/B3*100</f>
+        <v>104.39551308683008</v>
+      </c>
+      <c r="E39">
+        <f>E3/B3*100</f>
+        <v>104.05484004985459</v>
+      </c>
+      <c r="F39">
+        <f>F3/B3*100</f>
+        <v>103.9551308683008</v>
+      </c>
+      <c r="G39">
+        <f>G3/B3*100</f>
+        <v>103.82218529289572</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="7">
+        <v>1.804</v>
+      </c>
+      <c r="C40">
+        <f>C4/B4*100</f>
+        <v>91.44678492239467</v>
+      </c>
+      <c r="D40">
+        <f>D4/B4*100</f>
+        <v>91.44678492239467</v>
+      </c>
+      <c r="E40">
+        <f>E4/B4*100</f>
+        <v>91.396895787139684</v>
+      </c>
+      <c r="F40">
+        <f>F4/B4*100</f>
+        <v>91.402439024390247</v>
+      </c>
+      <c r="G40">
+        <f>G4/B4*100</f>
+        <v>91.380266075388022</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="7">
+        <v>0.37430000000000002</v>
+      </c>
+      <c r="C41">
+        <f>C5/B5*100</f>
+        <v>100.72134651349185</v>
+      </c>
+      <c r="D41">
+        <f>D5/B5*100</f>
+        <v>100.48089767566123</v>
+      </c>
+      <c r="E41">
+        <f>E5/B5*100</f>
+        <v>100.4541811381245</v>
+      </c>
+      <c r="F41">
+        <f>F5/B5*100</f>
+        <v>100.50761421319795</v>
+      </c>
+      <c r="G41">
+        <f>G5/B5*100</f>
+        <v>100.42746460058775</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="3">
+        <v>0</v>
+      </c>
+      <c r="C43" s="3">
+        <v>9</v>
+      </c>
+      <c r="D43" s="3">
+        <v>18</v>
+      </c>
+      <c r="E43" s="3">
+        <v>27</v>
+      </c>
+      <c r="F43" s="3">
+        <v>36</v>
+      </c>
+      <c r="G43" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="7">
+        <v>1.1283000000000001</v>
+      </c>
+      <c r="C44">
+        <f>C32/B32*100</f>
+        <v>100.21270938580165</v>
+      </c>
+      <c r="D44">
+        <f>D32/B32*100</f>
+        <v>100.27474962332712</v>
+      </c>
+      <c r="E44">
+        <f>E32/B32*100</f>
+        <v>100.31020118762738</v>
+      </c>
+      <c r="F44">
+        <f>F32/B32*100</f>
+        <v>100.32792696977752</v>
+      </c>
+      <c r="G44">
+        <f>G32/B32*100</f>
+        <v>100.34565275192769</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="7">
+        <v>1.2511000000000001</v>
+      </c>
+      <c r="C45">
+        <f>C33/B33*100</f>
+        <v>100.09591559427702</v>
+      </c>
+      <c r="D45">
+        <f>D33/B33*100</f>
+        <v>100.03996483094878</v>
+      </c>
+      <c r="E45">
+        <f>E33/B33*100</f>
+        <v>100.00799296618976</v>
+      </c>
+      <c r="F45">
+        <f>F33/B33*100</f>
+        <v>99.976021101430717</v>
+      </c>
+      <c r="G45">
+        <f>G33/B33*100</f>
+        <v>99.952042202861463</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="7">
+        <v>1.6489</v>
+      </c>
+      <c r="C46">
+        <f>C34/B34*100</f>
+        <v>99.939353508399535</v>
+      </c>
+      <c r="D46">
+        <f>D34/B34*100</f>
+        <v>99.933288859239482</v>
+      </c>
+      <c r="E46">
+        <f>E34/B34*100</f>
+        <v>99.890836315119174</v>
+      </c>
+      <c r="F46">
+        <f>F34/B34*100</f>
+        <v>99.957547455879677</v>
+      </c>
+      <c r="G46">
+        <f>G34/B34*100</f>
+        <v>99.927224210079444</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="7">
+        <v>0.37619999999999998</v>
+      </c>
+      <c r="C47">
+        <f>C35/B35*100</f>
+        <v>100.29239766081872</v>
+      </c>
+      <c r="D47">
+        <f>D35/B35*100</f>
+        <v>100.34556087187667</v>
+      </c>
+      <c r="E47">
+        <f>E35/B35*100</f>
+        <v>100.3189792663477</v>
+      </c>
+      <c r="F47">
+        <f t="array" ref="F47">F35/B35*100</f>
+        <v>100.3189792663477</v>
+      </c>
+      <c r="G47">
+        <f>G35/B35*100</f>
+        <v>100.3189792663477</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Added initial value for ipc and init graphs
</commit_message>
<xml_diff>
--- a/graphs/Project-Graphs.xlsx
+++ b/graphs/Project-Graphs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="899" firstSheet="5" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="899" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-anagram Before" sheetId="2" r:id="rId1"/>
@@ -6744,7 +6744,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="122" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="122" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -7969,8 +7969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8697,7 +8697,7 @@
         <v>8</v>
       </c>
       <c r="B38">
-        <v>1.1145</v>
+        <v>100</v>
       </c>
       <c r="C38">
         <f>C2/B2*100</f>
@@ -8724,8 +8724,8 @@
       <c r="A39" t="s">
         <v>9</v>
       </c>
-      <c r="B39" s="7">
-        <v>1.2035</v>
+      <c r="B39">
+        <v>100</v>
       </c>
       <c r="C39">
         <f>C3/B3*100</f>
@@ -8752,8 +8752,8 @@
       <c r="A40" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="7">
-        <v>1.804</v>
+      <c r="B40">
+        <v>100</v>
       </c>
       <c r="C40">
         <f>C4/B4*100</f>
@@ -8780,8 +8780,8 @@
       <c r="A41" t="s">
         <v>13</v>
       </c>
-      <c r="B41" s="7">
-        <v>0.37430000000000002</v>
+      <c r="B41">
+        <v>100</v>
       </c>
       <c r="C41">
         <f>C5/B5*100</f>
@@ -8832,7 +8832,7 @@
         <v>8</v>
       </c>
       <c r="B44" s="7">
-        <v>1.1283000000000001</v>
+        <v>100</v>
       </c>
       <c r="C44">
         <f>C32/B32*100</f>
@@ -8860,7 +8860,7 @@
         <v>9</v>
       </c>
       <c r="B45" s="7">
-        <v>1.2511000000000001</v>
+        <v>100</v>
       </c>
       <c r="C45">
         <f>C33/B33*100</f>
@@ -8888,7 +8888,7 @@
         <v>12</v>
       </c>
       <c r="B46" s="7">
-        <v>1.6489</v>
+        <v>100</v>
       </c>
       <c r="C46">
         <f>C34/B34*100</f>
@@ -8916,7 +8916,7 @@
         <v>13</v>
       </c>
       <c r="B47" s="7">
-        <v>0.37619999999999998</v>
+        <v>100</v>
       </c>
       <c r="C47">
         <f>C35/B35*100</f>

</xml_diff>